<commit_message>
collected ticks script separation
</commit_message>
<xml_diff>
--- a/data/raw-data/raw-ticks/collect/20240730_collect_tick.xlsx
+++ b/data/raw-data/raw-ticks/collect/20240730_collect_tick.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Feuil1!$A$1:$F$1</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -19,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="103">
   <si>
     <t>mission</t>
   </si>
@@ -680,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,16 +720,16 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>45824</v>
+        <v>45464</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C3" s="1">
         <v>45464</v>
@@ -743,7 +746,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -751,7 +754,7 @@
         <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C4" s="1">
         <v>45464</v>
@@ -768,7 +771,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C5" s="1">
         <v>45464</v>
@@ -785,7 +788,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>45464</v>
@@ -802,16 +805,16 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>45464</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -819,7 +822,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>45464</v>
@@ -836,16 +839,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="1">
-        <v>45464</v>
+        <v>45463</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -853,7 +856,7 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="C10" s="1">
         <v>45463</v>
@@ -861,19 +864,25 @@
       <c r="D10">
         <v>0</v>
       </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C11" s="1">
         <v>45463</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="F11" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -881,13 +890,16 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C12" s="1">
         <v>45463</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="F12" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -895,13 +907,16 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="C13" s="1">
         <v>45463</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="F13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -909,13 +924,16 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>29</v>
       </c>
       <c r="C14" s="1">
         <v>45463</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>10</v>
+      </c>
+      <c r="F14" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -923,7 +941,7 @@
         <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="C15" s="1">
         <v>45463</v>
@@ -931,22 +949,25 @@
       <c r="D15">
         <v>0</v>
       </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>7</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="C16" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D16">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -954,16 +975,16 @@
         <v>7</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C17" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -971,16 +992,16 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C18" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D18">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -988,16 +1009,16 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="C19" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D19">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1005,16 +1026,16 @@
         <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D20">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -1022,16 +1043,16 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="C21" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D21">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,16 +1060,16 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C22" s="1">
-        <v>45463</v>
+        <v>45461</v>
       </c>
       <c r="D22">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1056,16 +1077,16 @@
         <v>7</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C23" s="1">
         <v>45461</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1073,16 +1094,16 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="C24" s="1">
-        <v>45461</v>
+        <v>45460</v>
       </c>
       <c r="D24">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1090,16 +1111,16 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1">
-        <v>45461</v>
+        <v>45460</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1107,16 +1128,16 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="C26" s="1">
-        <v>45461</v>
+        <v>45460</v>
       </c>
       <c r="D26">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>39</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1124,16 +1145,16 @@
         <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>8</v>
       </c>
       <c r="C27" s="1">
-        <v>45461</v>
+        <v>45459</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1141,13 +1162,16 @@
         <v>7</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C28" s="1">
-        <v>45461</v>
+        <v>45458</v>
       </c>
       <c r="D28">
         <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1155,13 +1179,16 @@
         <v>7</v>
       </c>
       <c r="B29" t="s">
-        <v>42</v>
+        <v>53</v>
       </c>
       <c r="C29" s="1">
-        <v>45461</v>
+        <v>45458</v>
       </c>
       <c r="D29">
         <v>0</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1169,13 +1196,16 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>54</v>
       </c>
       <c r="C30" s="1">
-        <v>45461</v>
+        <v>45458</v>
       </c>
       <c r="D30">
         <v>0</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1183,13 +1213,16 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C31" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D31">
         <v>0</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1197,13 +1230,16 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C32" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D32">
         <v>0</v>
+      </c>
+      <c r="F32" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1211,13 +1247,16 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D33">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1225,13 +1264,16 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="C34" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1239,13 +1281,16 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C35" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D35">
         <v>0</v>
+      </c>
+      <c r="F35" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1253,13 +1298,16 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>44</v>
+        <v>62</v>
       </c>
       <c r="C36" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D36">
         <v>0</v>
+      </c>
+      <c r="F36" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1267,16 +1315,16 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C37" s="1">
-        <v>45460</v>
+        <v>45458</v>
       </c>
       <c r="D37">
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1284,16 +1332,16 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>65</v>
       </c>
       <c r="C38" s="1">
-        <v>45460</v>
+        <v>45455</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>34</v>
+        <v>75</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1301,16 +1349,16 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C39" s="1">
-        <v>45460</v>
+        <v>45455</v>
       </c>
       <c r="D39">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>45</v>
+        <v>67</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1318,16 +1366,16 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>68</v>
       </c>
       <c r="C40" s="1">
-        <v>45460</v>
+        <v>45455</v>
       </c>
       <c r="D40">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1335,16 +1383,16 @@
         <v>7</v>
       </c>
       <c r="B41" t="s">
-        <v>47</v>
+        <v>69</v>
       </c>
       <c r="C41" s="1">
-        <v>45460</v>
+        <v>45455</v>
       </c>
       <c r="D41">
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1352,16 +1400,16 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>70</v>
       </c>
       <c r="C42" s="1">
-        <v>45460</v>
+        <v>45455</v>
       </c>
       <c r="D42">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1369,16 +1417,16 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>51</v>
+        <v>71</v>
       </c>
       <c r="C43" s="1">
-        <v>45458</v>
+        <v>45455</v>
       </c>
       <c r="D43">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1386,13 +1434,16 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C44" s="1">
-        <v>45458</v>
+        <v>45455</v>
       </c>
       <c r="D44">
         <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1400,529 +1451,577 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C45" s="1">
-        <v>45458</v>
+        <v>45455</v>
       </c>
       <c r="D45">
         <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
       <c r="C46" s="1">
-        <v>45458</v>
+        <v>45224</v>
       </c>
       <c r="D46">
         <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="C47" s="1">
-        <v>45458</v>
+        <v>45224</v>
       </c>
       <c r="D47">
         <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="C48" s="1">
-        <v>45458</v>
+        <v>45224</v>
       </c>
       <c r="D48">
         <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B49" t="s">
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C49" s="1">
-        <v>45458</v>
+        <v>45224</v>
       </c>
       <c r="D49">
         <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B50" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C50" s="1">
-        <v>45458</v>
+        <v>45224</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B51" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C51" s="1">
-        <v>45458</v>
+        <v>45224</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>61</v>
+        <v>32</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B52" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="C52" s="1">
-        <v>45458</v>
+        <v>45223</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B53" t="s">
-        <v>63</v>
+        <v>44</v>
       </c>
       <c r="C53" s="1">
-        <v>45458</v>
+        <v>45223</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>64</v>
+        <v>76</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B54" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C54" s="1">
-        <v>45457</v>
+        <v>45223</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
-      <c r="F54" t="e">
-        <v>#N/A</v>
+      <c r="F54" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C55" s="1">
-        <v>45457</v>
+        <v>45223</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="C56" s="1">
-        <v>45457</v>
+        <v>45223</v>
       </c>
       <c r="D56">
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>55</v>
+        <v>77</v>
       </c>
       <c r="C57" s="1">
-        <v>45457</v>
+        <v>45223</v>
       </c>
       <c r="D57">
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>13</v>
+        <v>76</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B58" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C58" s="1">
-        <v>45457</v>
+        <v>45221</v>
       </c>
       <c r="D58">
         <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C59" s="1">
-        <v>45457</v>
+        <v>45221</v>
       </c>
       <c r="D59">
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>13</v>
+        <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C60" s="1">
-        <v>45457</v>
+        <v>45221</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>18</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>58</v>
+        <v>79</v>
       </c>
       <c r="C61" s="1">
-        <v>45457</v>
+        <v>45221</v>
       </c>
       <c r="D61">
         <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>63</v>
+        <v>8</v>
       </c>
       <c r="C62" s="1">
-        <v>45457</v>
+        <v>45221</v>
       </c>
       <c r="D62">
         <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C63" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D63">
         <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C64" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D64">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>67</v>
+        <v>78</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="C65" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D65">
         <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>68</v>
+        <v>16</v>
       </c>
       <c r="C66" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D66">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>69</v>
+        <v>17</v>
       </c>
       <c r="C67" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D67">
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>34</v>
+        <v>81</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
+        <v>19</v>
       </c>
       <c r="C68" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D68">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B69" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="C69" s="1">
-        <v>45455</v>
+        <v>45221</v>
       </c>
       <c r="D69">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>36</v>
+        <v>76</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B70" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="C70" s="1">
-        <v>45455</v>
+        <v>45216</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B71" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="C71" s="1">
-        <v>45455</v>
+        <v>45216</v>
       </c>
       <c r="D71">
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>65</v>
+        <v>10</v>
       </c>
       <c r="C72" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D72">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>75</v>
+        <v>85</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C73" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D73">
         <v>0</v>
+      </c>
+      <c r="F73" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C74" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D74">
         <v>0</v>
+      </c>
+      <c r="F74" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B75" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C75" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D75">
         <v>0</v>
+      </c>
+      <c r="F75" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B76" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C76" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D76">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="F76" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B77" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C77" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D77">
         <v>0</v>
+      </c>
+      <c r="F77" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B78" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C78" s="1">
-        <v>45454</v>
+        <v>45216</v>
       </c>
       <c r="D78">
         <v>0</v>
+      </c>
+      <c r="F78" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -1930,16 +2029,16 @@
         <v>2</v>
       </c>
       <c r="B79" t="s">
-        <v>12</v>
+        <v>71</v>
       </c>
       <c r="C79" s="1">
-        <v>45224</v>
+        <v>45216</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,16 +2046,16 @@
         <v>2</v>
       </c>
       <c r="B80" t="s">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="C80" s="1">
-        <v>45224</v>
+        <v>45216</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -1964,577 +2063,577 @@
         <v>2</v>
       </c>
       <c r="B81" t="s">
-        <v>33</v>
+        <v>74</v>
       </c>
       <c r="C81" s="1">
-        <v>45224</v>
+        <v>45216</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>32</v>
+        <v>84</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="C82" s="1">
-        <v>45224</v>
+        <v>45085</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>32</v>
+        <v>86</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="C83" s="1">
-        <v>45224</v>
+        <v>45085</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>32</v>
+        <v>87</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C84" s="1">
-        <v>45224</v>
+        <v>45085</v>
       </c>
       <c r="D84">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>32</v>
+        <v>88</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B85" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="C85" s="1">
-        <v>45223</v>
+        <v>45085</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>44</v>
+        <v>8</v>
       </c>
       <c r="C86" s="1">
-        <v>45223</v>
+        <v>45085</v>
       </c>
       <c r="D86">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C87" s="1">
-        <v>45223</v>
+        <v>45085</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="C88" s="1">
-        <v>45223</v>
+        <v>45085</v>
       </c>
       <c r="D88">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B89" t="s">
-        <v>43</v>
+        <v>12</v>
       </c>
       <c r="C89" s="1">
-        <v>45223</v>
+        <v>45085</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C90" s="1">
-        <v>45223</v>
+        <v>45085</v>
       </c>
       <c r="D90">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B91" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="C91" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C92" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D92">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B93" t="s">
-        <v>55</v>
+        <v>17</v>
       </c>
       <c r="C93" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>79</v>
+        <v>19</v>
       </c>
       <c r="C94" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B95" t="s">
-        <v>8</v>
+        <v>82</v>
       </c>
       <c r="C95" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D95">
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>56</v>
+        <v>33</v>
       </c>
       <c r="C96" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D96">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B97" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C97" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D97">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="F97" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C98" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>80</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B99" t="s">
-        <v>16</v>
+        <v>38</v>
       </c>
       <c r="C99" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D99">
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B100" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C100" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D100">
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>81</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B101" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="C101" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D101">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F101" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>82</v>
+        <v>41</v>
       </c>
       <c r="C102" s="1">
-        <v>45221</v>
+        <v>45085</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B103" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C103" s="1">
-        <v>45216</v>
+        <v>45081</v>
       </c>
       <c r="D103">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F103" t="s">
-        <v>83</v>
+        <v>94</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C104" s="1">
-        <v>45216</v>
+        <v>45081</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B105" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="C105" s="1">
-        <v>45216</v>
+        <v>45081</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C106" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D106">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="F106" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>68</v>
+        <v>51</v>
       </c>
       <c r="C107" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="F107" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="C108" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D108">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B109" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C109" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>24</v>
       </c>
       <c r="F109" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C110" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D110">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="F110" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B111" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C111" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D111">
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B112" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C112" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F112" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C113" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F113" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C114" s="1">
-        <v>45216</v>
+        <v>45078</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="F114" t="s">
-        <v>84</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -2542,13 +2641,16 @@
         <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="C115" s="1">
-        <v>45085</v>
+        <v>45078</v>
       </c>
       <c r="D115">
         <v>0</v>
+      </c>
+      <c r="F115" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -2556,1073 +2658,228 @@
         <v>3</v>
       </c>
       <c r="B116" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C116" s="1">
-        <v>45085</v>
+        <v>45078</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>19</v>
+      </c>
+      <c r="F116" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
-        <v>3</v>
-      </c>
-      <c r="B117" t="s">
-        <v>55</v>
-      </c>
-      <c r="C117" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D117">
-        <v>0</v>
-      </c>
+      <c r="C117" s="1"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>3</v>
-      </c>
-      <c r="B118" t="s">
-        <v>79</v>
-      </c>
-      <c r="C118" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D118">
-        <v>0</v>
-      </c>
+      <c r="C118" s="1"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>3</v>
-      </c>
-      <c r="B119" t="s">
-        <v>8</v>
-      </c>
-      <c r="C119" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D119">
-        <v>0</v>
-      </c>
+      <c r="C119" s="1"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
-        <v>3</v>
-      </c>
-      <c r="B120" t="s">
-        <v>56</v>
-      </c>
-      <c r="C120" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D120">
-        <v>0</v>
-      </c>
+      <c r="C120" s="1"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
-        <v>3</v>
-      </c>
-      <c r="B121" t="s">
-        <v>57</v>
-      </c>
-      <c r="C121" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D121">
-        <v>0</v>
-      </c>
+      <c r="C121" s="1"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
-        <v>3</v>
-      </c>
-      <c r="B122" t="s">
-        <v>12</v>
-      </c>
-      <c r="C122" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D122">
-        <v>0</v>
-      </c>
+      <c r="C122" s="1"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
-        <v>3</v>
-      </c>
-      <c r="B123" t="s">
-        <v>14</v>
-      </c>
-      <c r="C123" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D123">
-        <v>0</v>
-      </c>
+      <c r="C123" s="1"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
-        <v>3</v>
-      </c>
-      <c r="B124" t="s">
-        <v>15</v>
-      </c>
-      <c r="C124" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D124">
-        <v>0</v>
-      </c>
+      <c r="C124" s="1"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
-        <v>3</v>
-      </c>
-      <c r="B125" t="s">
-        <v>16</v>
-      </c>
-      <c r="C125" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D125">
-        <v>0</v>
-      </c>
+      <c r="C125" s="1"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
-        <v>3</v>
-      </c>
-      <c r="B126" t="s">
-        <v>17</v>
-      </c>
-      <c r="C126" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D126">
-        <v>0</v>
-      </c>
+      <c r="C126" s="1"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
-        <v>3</v>
-      </c>
-      <c r="B127" t="s">
-        <v>19</v>
-      </c>
-      <c r="C127" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D127">
-        <v>0</v>
-      </c>
+      <c r="C127" s="1"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>3</v>
-      </c>
-      <c r="B128" t="s">
-        <v>82</v>
-      </c>
-      <c r="C128" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D128">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>3</v>
-      </c>
-      <c r="B129" t="s">
-        <v>33</v>
-      </c>
-      <c r="C129" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D129">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
-        <v>3</v>
-      </c>
-      <c r="B130" t="s">
-        <v>35</v>
-      </c>
-      <c r="C130" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D130">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
-        <v>3</v>
-      </c>
-      <c r="B131" t="s">
-        <v>37</v>
-      </c>
-      <c r="C131" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D131">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
-        <v>3</v>
-      </c>
-      <c r="B132" t="s">
-        <v>38</v>
-      </c>
-      <c r="C132" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D132">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>3</v>
-      </c>
-      <c r="B133" t="s">
-        <v>40</v>
-      </c>
-      <c r="C133" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D133">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
-        <v>3</v>
-      </c>
-      <c r="B134" t="s">
-        <v>44</v>
-      </c>
-      <c r="C134" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D134">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>3</v>
-      </c>
-      <c r="B135" t="s">
-        <v>41</v>
-      </c>
-      <c r="C135" s="1">
-        <v>45085</v>
-      </c>
-      <c r="D135">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
-        <v>3</v>
-      </c>
-      <c r="B136" t="s">
-        <v>53</v>
-      </c>
-      <c r="C136" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D136">
-        <v>0</v>
-      </c>
-      <c r="F136" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
-        <v>3</v>
-      </c>
-      <c r="B137" t="s">
-        <v>54</v>
-      </c>
-      <c r="C137" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D137">
-        <v>0</v>
-      </c>
-      <c r="F137" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
-        <v>3</v>
-      </c>
-      <c r="B138" t="s">
-        <v>55</v>
-      </c>
-      <c r="C138" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D138">
-        <v>7</v>
-      </c>
-      <c r="F138" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
-        <v>3</v>
-      </c>
-      <c r="B139" t="s">
-        <v>79</v>
-      </c>
-      <c r="C139" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D139">
-        <v>0</v>
-      </c>
-      <c r="F139" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
-        <v>3</v>
-      </c>
-      <c r="B140" t="s">
-        <v>8</v>
-      </c>
-      <c r="C140" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D140">
-        <v>1</v>
-      </c>
-      <c r="F140" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>3</v>
-      </c>
-      <c r="B141" t="s">
-        <v>56</v>
-      </c>
-      <c r="C141" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D141">
-        <v>0</v>
-      </c>
-      <c r="F141" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A142" t="s">
-        <v>3</v>
-      </c>
-      <c r="B142" t="s">
-        <v>57</v>
-      </c>
-      <c r="C142" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D142">
-        <v>1</v>
-      </c>
-      <c r="F142" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A143" t="s">
-        <v>3</v>
-      </c>
-      <c r="B143" t="s">
-        <v>15</v>
-      </c>
-      <c r="C143" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D143">
-        <v>0</v>
-      </c>
-      <c r="F143" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
-        <v>3</v>
-      </c>
-      <c r="B144" t="s">
-        <v>16</v>
-      </c>
-      <c r="C144" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D144">
-        <v>1</v>
-      </c>
-      <c r="F144" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
-        <v>3</v>
-      </c>
-      <c r="B145" t="s">
-        <v>17</v>
-      </c>
-      <c r="C145" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D145">
-        <v>0</v>
-      </c>
-      <c r="F145" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A146" t="s">
-        <v>3</v>
-      </c>
-      <c r="B146" t="s">
-        <v>19</v>
-      </c>
-      <c r="C146" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D146">
-        <v>0</v>
-      </c>
-      <c r="F146" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A147" t="s">
-        <v>3</v>
-      </c>
-      <c r="B147" t="s">
-        <v>82</v>
-      </c>
-      <c r="C147" s="1">
-        <v>45084</v>
-      </c>
-      <c r="D147">
-        <v>0</v>
-      </c>
-      <c r="F147" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>3</v>
-      </c>
-      <c r="B148" t="s">
-        <v>12</v>
-      </c>
-      <c r="C148" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D148">
-        <v>0</v>
-      </c>
-      <c r="F148" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
-        <v>3</v>
-      </c>
-      <c r="B149" t="s">
-        <v>14</v>
-      </c>
-      <c r="C149" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D149">
-        <v>1</v>
-      </c>
-      <c r="F149" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
-        <v>3</v>
-      </c>
-      <c r="B150" t="s">
-        <v>33</v>
-      </c>
-      <c r="C150" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D150">
-        <v>1</v>
-      </c>
-      <c r="F150" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
-        <v>3</v>
-      </c>
-      <c r="B151" t="s">
-        <v>35</v>
-      </c>
-      <c r="C151" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D151">
-        <v>9</v>
-      </c>
-      <c r="F151" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A152" t="s">
-        <v>3</v>
-      </c>
-      <c r="B152" t="s">
-        <v>37</v>
-      </c>
-      <c r="C152" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D152">
-        <v>0</v>
-      </c>
-      <c r="F152" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A153" t="s">
-        <v>3</v>
-      </c>
-      <c r="B153" t="s">
-        <v>38</v>
-      </c>
-      <c r="C153" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D153">
-        <v>0</v>
-      </c>
-      <c r="F153" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A154" t="s">
-        <v>3</v>
-      </c>
-      <c r="B154" t="s">
-        <v>40</v>
-      </c>
-      <c r="C154" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D154">
-        <v>1</v>
-      </c>
-      <c r="F154" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
-        <v>3</v>
-      </c>
-      <c r="B155" t="s">
-        <v>44</v>
-      </c>
-      <c r="C155" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D155">
-        <v>6</v>
-      </c>
-      <c r="F155" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
-        <v>3</v>
-      </c>
-      <c r="B156" t="s">
-        <v>41</v>
-      </c>
-      <c r="C156" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D156">
-        <v>0</v>
-      </c>
-      <c r="F156" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A157" t="s">
-        <v>3</v>
-      </c>
-      <c r="B157" t="s">
-        <v>42</v>
-      </c>
-      <c r="C157" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D157">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>3</v>
-      </c>
-      <c r="B158" t="s">
-        <v>43</v>
-      </c>
-      <c r="C158" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D158">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
-        <v>3</v>
-      </c>
-      <c r="B159" t="s">
-        <v>77</v>
-      </c>
-      <c r="C159" s="1">
-        <v>45081</v>
-      </c>
-      <c r="D159">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
-        <v>3</v>
-      </c>
-      <c r="B160" t="s">
-        <v>42</v>
-      </c>
-      <c r="C160" s="1">
-        <v>45080</v>
-      </c>
-      <c r="D160">
-        <v>6</v>
-      </c>
-      <c r="F160" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>3</v>
-      </c>
-      <c r="B161" t="s">
-        <v>43</v>
-      </c>
-      <c r="C161" s="1">
-        <v>45080</v>
-      </c>
-      <c r="D161">
-        <v>0</v>
-      </c>
-      <c r="F161" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>3</v>
-      </c>
-      <c r="B162" t="s">
-        <v>77</v>
-      </c>
-      <c r="C162" s="1">
-        <v>45080</v>
-      </c>
-      <c r="D162">
-        <v>0</v>
-      </c>
-      <c r="F162" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" t="s">
-        <v>3</v>
-      </c>
-      <c r="B163" t="s">
-        <v>65</v>
-      </c>
-      <c r="C163" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
-        <v>3</v>
-      </c>
-      <c r="B164" t="s">
-        <v>51</v>
-      </c>
-      <c r="C164" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D164">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" t="s">
-        <v>3</v>
-      </c>
-      <c r="B165" t="s">
-        <v>10</v>
-      </c>
-      <c r="C165" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D165">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" t="s">
-        <v>3</v>
-      </c>
-      <c r="B166" t="s">
-        <v>66</v>
-      </c>
-      <c r="C166" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A167" t="s">
-        <v>3</v>
-      </c>
-      <c r="B167" t="s">
-        <v>68</v>
-      </c>
-      <c r="C167" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D167">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A168" t="s">
-        <v>3</v>
-      </c>
-      <c r="B168" t="s">
-        <v>58</v>
-      </c>
-      <c r="C168" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D168">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A169" t="s">
-        <v>3</v>
-      </c>
-      <c r="B169" t="s">
-        <v>69</v>
-      </c>
-      <c r="C169" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D169">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A170" t="s">
-        <v>3</v>
-      </c>
-      <c r="B170" t="s">
-        <v>70</v>
-      </c>
-      <c r="C170" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D170">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A171" t="s">
-        <v>3</v>
-      </c>
-      <c r="B171" t="s">
-        <v>70</v>
-      </c>
-      <c r="C171" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D171">
-        <v>2</v>
-      </c>
-      <c r="F171" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A172" t="s">
-        <v>3</v>
-      </c>
-      <c r="B172" t="s">
-        <v>71</v>
-      </c>
-      <c r="C172" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D172">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A173" t="s">
-        <v>3</v>
-      </c>
-      <c r="B173" t="s">
-        <v>72</v>
-      </c>
-      <c r="C173" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D173">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A174" t="s">
-        <v>3</v>
-      </c>
-      <c r="B174" t="s">
-        <v>74</v>
-      </c>
-      <c r="C174" s="1">
-        <v>45078</v>
-      </c>
-      <c r="D174">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A175" t="s">
-        <v>3</v>
-      </c>
-      <c r="B175" t="s">
-        <v>65</v>
-      </c>
-      <c r="C175" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D175">
-        <v>20</v>
-      </c>
-      <c r="F175" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A176" t="s">
-        <v>3</v>
-      </c>
-      <c r="B176" t="s">
-        <v>51</v>
-      </c>
-      <c r="C176" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D176">
-        <v>0</v>
-      </c>
-      <c r="F176" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A177" t="s">
-        <v>3</v>
-      </c>
-      <c r="B177" t="s">
-        <v>10</v>
-      </c>
-      <c r="C177" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D177">
-        <v>1</v>
-      </c>
-      <c r="F177" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A178" t="s">
-        <v>3</v>
-      </c>
-      <c r="B178" t="s">
-        <v>66</v>
-      </c>
-      <c r="C178" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D178">
-        <v>24</v>
-      </c>
-      <c r="F178" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A179" t="s">
-        <v>3</v>
-      </c>
-      <c r="B179" t="s">
-        <v>68</v>
-      </c>
-      <c r="C179" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D179">
-        <v>12</v>
-      </c>
-      <c r="F179" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
-        <v>3</v>
-      </c>
-      <c r="B180" t="s">
-        <v>58</v>
-      </c>
-      <c r="C180" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D180">
-        <v>0</v>
-      </c>
-      <c r="F180" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A181" t="s">
-        <v>3</v>
-      </c>
-      <c r="B181" t="s">
-        <v>69</v>
-      </c>
-      <c r="C181" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D181">
-        <v>8</v>
-      </c>
-      <c r="F181" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A182" t="s">
-        <v>3</v>
-      </c>
-      <c r="B182" t="s">
-        <v>71</v>
-      </c>
-      <c r="C182" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D182">
-        <v>21</v>
-      </c>
-      <c r="F182" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A183" t="s">
-        <v>3</v>
-      </c>
-      <c r="B183" t="s">
-        <v>72</v>
-      </c>
-      <c r="C183" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D183">
-        <v>0</v>
-      </c>
-      <c r="F183" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A184" t="s">
-        <v>3</v>
-      </c>
-      <c r="B184" t="s">
-        <v>74</v>
-      </c>
-      <c r="C184" s="1">
-        <v>45077</v>
-      </c>
-      <c r="D184">
-        <v>19</v>
-      </c>
-      <c r="F184" t="s">
-        <v>101</v>
-      </c>
+      <c r="C128" s="1"/>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="1"/>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="1"/>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="1"/>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="1"/>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="1"/>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="1"/>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="1"/>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="1"/>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="1"/>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="1"/>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="1"/>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="1"/>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="1"/>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="1"/>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="1"/>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="1"/>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="1"/>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="1"/>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="1"/>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="1"/>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="1"/>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="1"/>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="1"/>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="1"/>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="1"/>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="1"/>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="1"/>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="1"/>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="1"/>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="1"/>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="1"/>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C160" s="1"/>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="1"/>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="1"/>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="1"/>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="1"/>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="1"/>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="1"/>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="1"/>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="1"/>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="1"/>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="1"/>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="1"/>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="1"/>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="1"/>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174" s="1"/>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="1"/>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="1"/>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="1"/>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="1"/>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="1"/>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="1"/>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="1"/>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="1"/>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="1"/>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="1"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:F1">
+    <sortState ref="A2:F184">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
After restoring (i'm alive)
I loose 1 week of code, rewritten it during weekedn super
</commit_message>
<xml_diff>
--- a/data/raw-data/raw-ticks/collect/20240730_collect_tick.xlsx
+++ b/data/raw-data/raw-ticks/collect/20240730_collect_tick.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B941F0B4-F8CD-4B09-9448-CDAF6968B9CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,9 +25,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="103">
   <si>
-    <t>mission</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
@@ -34,12 +32,6 @@
   </si>
   <si>
     <t>FRA - BePrep - Juin 2023</t>
-  </si>
-  <si>
-    <t>line</t>
-  </si>
-  <si>
-    <t>tick_number</t>
   </si>
   <si>
     <t>weather</t>
@@ -360,12 +352,21 @@
   </si>
   <si>
     <t>comment</t>
+  </si>
+  <si>
+    <t>code_mission</t>
+  </si>
+  <si>
+    <t>numero_ligne</t>
+  </si>
+  <si>
+    <t>effectif_tick</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
   </numFmts>
@@ -680,11 +681,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F184"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:F25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -697,30 +698,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>101</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
       </c>
       <c r="C2" s="1">
         <v>45464</v>
@@ -729,15 +730,15 @@
         <v>0</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>45464</v>
@@ -746,15 +747,15 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>45464</v>
@@ -763,15 +764,15 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>45464</v>
@@ -780,15 +781,15 @@
         <v>0</v>
       </c>
       <c r="F5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C6" s="1">
         <v>45464</v>
@@ -797,15 +798,15 @@
         <v>0</v>
       </c>
       <c r="F6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C7" s="1">
         <v>45464</v>
@@ -814,15 +815,15 @@
         <v>1</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C8" s="1">
         <v>45464</v>
@@ -831,15 +832,15 @@
         <v>1</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C9" s="1">
         <v>45463</v>
@@ -848,15 +849,15 @@
         <v>3</v>
       </c>
       <c r="F9" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C10" s="1">
         <v>45463</v>
@@ -865,15 +866,15 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C11" s="1">
         <v>45463</v>
@@ -882,15 +883,15 @@
         <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C12" s="1">
         <v>45463</v>
@@ -899,15 +900,15 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C13" s="1">
         <v>45463</v>
@@ -916,15 +917,15 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C14" s="1">
         <v>45463</v>
@@ -933,15 +934,15 @@
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C15" s="1">
         <v>45463</v>
@@ -950,15 +951,15 @@
         <v>0</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C16" s="1">
         <v>45461</v>
@@ -967,15 +968,15 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C17" s="1">
         <v>45461</v>
@@ -984,15 +985,15 @@
         <v>3</v>
       </c>
       <c r="F17" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18" s="1">
         <v>45461</v>
@@ -1001,15 +1002,15 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19" s="1">
         <v>45461</v>
@@ -1018,15 +1019,15 @@
         <v>5</v>
       </c>
       <c r="F19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C20" s="1">
         <v>45461</v>
@@ -1035,15 +1036,15 @@
         <v>1</v>
       </c>
       <c r="F20" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C21" s="1">
         <v>45461</v>
@@ -1052,15 +1053,15 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C22" s="1">
         <v>45461</v>
@@ -1069,15 +1070,15 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C23" s="1">
         <v>45461</v>
@@ -1086,15 +1087,15 @@
         <v>0</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C24" s="1">
         <v>45460</v>
@@ -1103,15 +1104,15 @@
         <v>1</v>
       </c>
       <c r="F24" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="C25" s="1">
         <v>45460</v>
@@ -1120,15 +1121,15 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1">
         <v>45460</v>
@@ -1137,15 +1138,15 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B27" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C27" s="1">
         <v>45459</v>
@@ -1154,15 +1155,15 @@
         <v>2</v>
       </c>
       <c r="F27" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B28" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C28" s="1">
         <v>45458</v>
@@ -1171,15 +1172,15 @@
         <v>0</v>
       </c>
       <c r="F28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B29" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C29" s="1">
         <v>45458</v>
@@ -1188,15 +1189,15 @@
         <v>0</v>
       </c>
       <c r="F29" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C30" s="1">
         <v>45458</v>
@@ -1205,15 +1206,15 @@
         <v>0</v>
       </c>
       <c r="F30" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C31" s="1">
         <v>45458</v>
@@ -1222,15 +1223,15 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C32" s="1">
         <v>45458</v>
@@ -1239,15 +1240,15 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B33" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C33" s="1">
         <v>45458</v>
@@ -1256,15 +1257,15 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B34" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C34" s="1">
         <v>45458</v>
@@ -1273,15 +1274,15 @@
         <v>1</v>
       </c>
       <c r="F34" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C35" s="1">
         <v>45458</v>
@@ -1290,15 +1291,15 @@
         <v>0</v>
       </c>
       <c r="F35" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B36" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C36" s="1">
         <v>45458</v>
@@ -1307,15 +1308,15 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B37" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C37" s="1">
         <v>45458</v>
@@ -1324,15 +1325,15 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B38" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C38" s="1">
         <v>45455</v>
@@ -1341,15 +1342,15 @@
         <v>4</v>
       </c>
       <c r="F38" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C39" s="1">
         <v>45455</v>
@@ -1358,15 +1359,15 @@
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B40" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C40" s="1">
         <v>45455</v>
@@ -1375,15 +1376,15 @@
         <v>5</v>
       </c>
       <c r="F40" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C41" s="1">
         <v>45455</v>
@@ -1392,15 +1393,15 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C42" s="1">
         <v>45455</v>
@@ -1409,15 +1410,15 @@
         <v>3</v>
       </c>
       <c r="F42" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B43" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C43" s="1">
         <v>45455</v>
@@ -1426,15 +1427,15 @@
         <v>3</v>
       </c>
       <c r="F43" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B44" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C44" s="1">
         <v>45455</v>
@@ -1443,15 +1444,15 @@
         <v>0</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B45" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C45" s="1">
         <v>45455</v>
@@ -1460,15 +1461,15 @@
         <v>0</v>
       </c>
       <c r="F45" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C46" s="1">
         <v>45224</v>
@@ -1477,15 +1478,15 @@
         <v>0</v>
       </c>
       <c r="F46" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C47" s="1">
         <v>45224</v>
@@ -1494,15 +1495,15 @@
         <v>0</v>
       </c>
       <c r="F47" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B48" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C48" s="1">
         <v>45224</v>
@@ -1511,15 +1512,15 @@
         <v>0</v>
       </c>
       <c r="F48" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B49" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C49" s="1">
         <v>45224</v>
@@ -1528,15 +1529,15 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C50" s="1">
         <v>45224</v>
@@ -1545,15 +1546,15 @@
         <v>0</v>
       </c>
       <c r="F50" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C51" s="1">
         <v>45224</v>
@@ -1562,15 +1563,15 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B52" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C52" s="1">
         <v>45223</v>
@@ -1579,15 +1580,15 @@
         <v>0</v>
       </c>
       <c r="F52" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C53" s="1">
         <v>45223</v>
@@ -1596,15 +1597,15 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C54" s="1">
         <v>45223</v>
@@ -1613,15 +1614,15 @@
         <v>0</v>
       </c>
       <c r="F54" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C55" s="1">
         <v>45223</v>
@@ -1630,15 +1631,15 @@
         <v>0</v>
       </c>
       <c r="F55" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B56" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C56" s="1">
         <v>45223</v>
@@ -1647,15 +1648,15 @@
         <v>0</v>
       </c>
       <c r="F56" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B57" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C57" s="1">
         <v>45223</v>
@@ -1664,15 +1665,15 @@
         <v>0</v>
       </c>
       <c r="F57" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C58" s="1">
         <v>45221</v>
@@ -1681,15 +1682,15 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C59" s="1">
         <v>45221</v>
@@ -1698,15 +1699,15 @@
         <v>0</v>
       </c>
       <c r="F59" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B60" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C60" s="1">
         <v>45221</v>
@@ -1715,15 +1716,15 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B61" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C61" s="1">
         <v>45221</v>
@@ -1732,15 +1733,15 @@
         <v>0</v>
       </c>
       <c r="F61" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B62" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C62" s="1">
         <v>45221</v>
@@ -1749,15 +1750,15 @@
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C63" s="1">
         <v>45221</v>
@@ -1766,15 +1767,15 @@
         <v>0</v>
       </c>
       <c r="F63" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B64" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C64" s="1">
         <v>45221</v>
@@ -1783,15 +1784,15 @@
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B65" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C65" s="1">
         <v>45221</v>
@@ -1800,15 +1801,15 @@
         <v>0</v>
       </c>
       <c r="F65" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B66" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C66" s="1">
         <v>45221</v>
@@ -1817,15 +1818,15 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B67" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C67" s="1">
         <v>45221</v>
@@ -1834,15 +1835,15 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C68" s="1">
         <v>45221</v>
@@ -1851,15 +1852,15 @@
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C69" s="1">
         <v>45221</v>
@@ -1868,15 +1869,15 @@
         <v>0</v>
       </c>
       <c r="F69" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C70" s="1">
         <v>45216</v>
@@ -1885,15 +1886,15 @@
         <v>2</v>
       </c>
       <c r="F70" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C71" s="1">
         <v>45216</v>
@@ -1902,15 +1903,15 @@
         <v>0</v>
       </c>
       <c r="F71" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C72" s="1">
         <v>45216</v>
@@ -1919,15 +1920,15 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C73" s="1">
         <v>45216</v>
@@ -1936,15 +1937,15 @@
         <v>0</v>
       </c>
       <c r="F73" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C74" s="1">
         <v>45216</v>
@@ -1953,15 +1954,15 @@
         <v>0</v>
       </c>
       <c r="F74" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C75" s="1">
         <v>45216</v>
@@ -1970,15 +1971,15 @@
         <v>0</v>
       </c>
       <c r="F75" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C76" s="1">
         <v>45216</v>
@@ -1987,15 +1988,15 @@
         <v>1</v>
       </c>
       <c r="F76" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C77" s="1">
         <v>45216</v>
@@ -2004,15 +2005,15 @@
         <v>0</v>
       </c>
       <c r="F77" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C78" s="1">
         <v>45216</v>
@@ -2021,15 +2022,15 @@
         <v>0</v>
       </c>
       <c r="F78" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C79" s="1">
         <v>45216</v>
@@ -2038,15 +2039,15 @@
         <v>0</v>
       </c>
       <c r="F79" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C80" s="1">
         <v>45216</v>
@@ -2055,15 +2056,15 @@
         <v>0</v>
       </c>
       <c r="F80" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C81" s="1">
         <v>45216</v>
@@ -2072,15 +2073,15 @@
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B82" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C82" s="1">
         <v>45085</v>
@@ -2089,15 +2090,15 @@
         <v>0</v>
       </c>
       <c r="F82" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B83" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C83" s="1">
         <v>45085</v>
@@ -2106,15 +2107,15 @@
         <v>0</v>
       </c>
       <c r="F83" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B84" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C84" s="1">
         <v>45085</v>
@@ -2123,15 +2124,15 @@
         <v>7</v>
       </c>
       <c r="F84" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B85" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C85" s="1">
         <v>45085</v>
@@ -2140,15 +2141,15 @@
         <v>0</v>
       </c>
       <c r="F85" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B86" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C86" s="1">
         <v>45085</v>
@@ -2157,15 +2158,15 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B87" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C87" s="1">
         <v>45085</v>
@@ -2174,15 +2175,15 @@
         <v>0</v>
       </c>
       <c r="F87" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B88" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C88" s="1">
         <v>45085</v>
@@ -2191,15 +2192,15 @@
         <v>1</v>
       </c>
       <c r="F88" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B89" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C89" s="1">
         <v>45085</v>
@@ -2208,15 +2209,15 @@
         <v>0</v>
       </c>
       <c r="F89" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B90" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C90" s="1">
         <v>45085</v>
@@ -2225,15 +2226,15 @@
         <v>1</v>
       </c>
       <c r="F90" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B91" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C91" s="1">
         <v>45085</v>
@@ -2242,15 +2243,15 @@
         <v>0</v>
       </c>
       <c r="F91" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B92" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C92" s="1">
         <v>45085</v>
@@ -2259,15 +2260,15 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B93" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C93" s="1">
         <v>45085</v>
@@ -2276,15 +2277,15 @@
         <v>0</v>
       </c>
       <c r="F93" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B94" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C94" s="1">
         <v>45085</v>
@@ -2293,15 +2294,15 @@
         <v>0</v>
       </c>
       <c r="F94" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C95" s="1">
         <v>45085</v>
@@ -2310,15 +2311,15 @@
         <v>0</v>
       </c>
       <c r="F95" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B96" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C96" s="1">
         <v>45085</v>
@@ -2327,15 +2328,15 @@
         <v>1</v>
       </c>
       <c r="F96" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B97" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C97" s="1">
         <v>45085</v>
@@ -2344,15 +2345,15 @@
         <v>9</v>
       </c>
       <c r="F97" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B98" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C98" s="1">
         <v>45085</v>
@@ -2361,15 +2362,15 @@
         <v>0</v>
       </c>
       <c r="F98" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B99" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C99" s="1">
         <v>45085</v>
@@ -2378,15 +2379,15 @@
         <v>0</v>
       </c>
       <c r="F99" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B100" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C100" s="1">
         <v>45085</v>
@@ -2395,15 +2396,15 @@
         <v>1</v>
       </c>
       <c r="F100" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B101" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C101" s="1">
         <v>45085</v>
@@ -2412,15 +2413,15 @@
         <v>6</v>
       </c>
       <c r="F101" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B102" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C102" s="1">
         <v>45085</v>
@@ -2429,15 +2430,15 @@
         <v>0</v>
       </c>
       <c r="F102" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B103" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C103" s="1">
         <v>45081</v>
@@ -2446,15 +2447,15 @@
         <v>6</v>
       </c>
       <c r="F103" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B104" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C104" s="1">
         <v>45081</v>
@@ -2463,15 +2464,15 @@
         <v>0</v>
       </c>
       <c r="F104" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B105" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C105" s="1">
         <v>45081</v>
@@ -2480,15 +2481,15 @@
         <v>0</v>
       </c>
       <c r="F105" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B106" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C106" s="1">
         <v>45078</v>
@@ -2497,15 +2498,15 @@
         <v>20</v>
       </c>
       <c r="F106" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B107" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C107" s="1">
         <v>45078</v>
@@ -2514,15 +2515,15 @@
         <v>0</v>
       </c>
       <c r="F107" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B108" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C108" s="1">
         <v>45078</v>
@@ -2531,15 +2532,15 @@
         <v>1</v>
       </c>
       <c r="F108" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B109" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C109" s="1">
         <v>45078</v>
@@ -2548,15 +2549,15 @@
         <v>24</v>
       </c>
       <c r="F109" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B110" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C110" s="1">
         <v>45078</v>
@@ -2565,15 +2566,15 @@
         <v>12</v>
       </c>
       <c r="F110" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B111" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C111" s="1">
         <v>45078</v>
@@ -2582,15 +2583,15 @@
         <v>0</v>
       </c>
       <c r="F111" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B112" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C112" s="1">
         <v>45078</v>
@@ -2599,15 +2600,15 @@
         <v>8</v>
       </c>
       <c r="F112" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B113" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C113" s="1">
         <v>45078</v>
@@ -2616,15 +2617,15 @@
         <v>2</v>
       </c>
       <c r="F113" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B114" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C114" s="1">
         <v>45078</v>
@@ -2633,15 +2634,15 @@
         <v>21</v>
       </c>
       <c r="F114" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B115" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C115" s="1">
         <v>45078</v>
@@ -2650,15 +2651,15 @@
         <v>0</v>
       </c>
       <c r="F115" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B116" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C116" s="1">
         <v>45078</v>
@@ -2667,7 +2668,7 @@
         <v>19</v>
       </c>
       <c r="F116" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -2875,8 +2876,8 @@
       <c r="C184" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F1">
-    <sortState ref="A2:F184">
+  <autoFilter ref="A1:F1" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F184">
       <sortCondition ref="B1"/>
     </sortState>
   </autoFilter>

</xml_diff>